<commit_message>
practice past contest ABC129
</commit_message>
<xml_diff>
--- a/AtCoder_record.xlsx
+++ b/AtCoder_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\codes\AtCoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA58222-19D7-4EB9-8BB6-3BC8280C25EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4613EB4-035F-46D1-996E-793A22EE7FE2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11565" yWindow="3795" windowWidth="15255" windowHeight="15885" xr2:uid="{9B9A1409-A6B9-4D33-8F83-A064BA4B158C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="29">
   <si>
     <t>contest</t>
     <phoneticPr fontId="1"/>
@@ -190,6 +190,14 @@
     <rPh sb="3" eb="4">
       <t>ホウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dfs, dag</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -568,11 +576,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C233B7-3D4E-4872-A3EB-9A4A81938CC3}">
-  <dimension ref="A1:G121"/>
+  <dimension ref="A1:G128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F122" sqref="F122"/>
+      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G129" sqref="G129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2338,6 +2346,113 @@
       </c>
       <c r="F121" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A122">
+        <v>139</v>
+      </c>
+      <c r="B122" t="s">
+        <v>5</v>
+      </c>
+      <c r="C122" t="s">
+        <v>8</v>
+      </c>
+      <c r="E122" s="2">
+        <v>43709</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A123">
+        <v>139</v>
+      </c>
+      <c r="B123" t="s">
+        <v>6</v>
+      </c>
+      <c r="C123" t="s">
+        <v>8</v>
+      </c>
+      <c r="E123" s="2">
+        <v>43709</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A124">
+        <v>139</v>
+      </c>
+      <c r="B124" t="s">
+        <v>15</v>
+      </c>
+      <c r="C124" t="s">
+        <v>8</v>
+      </c>
+      <c r="E124" s="2">
+        <v>43709</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A125">
+        <v>139</v>
+      </c>
+      <c r="B125" t="s">
+        <v>19</v>
+      </c>
+      <c r="C125" t="s">
+        <v>8</v>
+      </c>
+      <c r="E125" s="2">
+        <v>43709</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A126">
+        <v>139</v>
+      </c>
+      <c r="B126" t="s">
+        <v>27</v>
+      </c>
+      <c r="C126" t="s">
+        <v>8</v>
+      </c>
+      <c r="D126" t="b">
+        <v>1</v>
+      </c>
+      <c r="E126" s="2">
+        <v>43710</v>
+      </c>
+      <c r="F126" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A127">
+        <v>129</v>
+      </c>
+      <c r="B127" t="s">
+        <v>19</v>
+      </c>
+      <c r="C127" t="s">
+        <v>8</v>
+      </c>
+      <c r="E127" s="2">
+        <v>43710</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A128">
+        <v>129</v>
+      </c>
+      <c r="B128" t="s">
+        <v>27</v>
+      </c>
+      <c r="C128" t="s">
+        <v>8</v>
+      </c>
+      <c r="E128" s="2">
+        <v>43710</v>
+      </c>
+      <c r="F128" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
done ABC105_D in plain sweep method
</commit_message>
<xml_diff>
--- a/AtCoder_record.xlsx
+++ b/AtCoder_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\codes\AtCoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF9CC4E-0557-417B-9303-FDE5D85E2DFC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDF5AC6-7190-4494-BACC-4FA8DA9A1AD4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11565" yWindow="3795" windowWidth="15255" windowHeight="15885" xr2:uid="{9B9A1409-A6B9-4D33-8F83-A064BA4B158C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="32">
   <si>
     <t>contest</t>
     <phoneticPr fontId="1"/>
@@ -204,6 +204,29 @@
     <t>逆元</t>
     <rPh sb="0" eb="2">
       <t>ギャクゲン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>二次元累積和</t>
+    <rPh sb="0" eb="3">
+      <t>ニジゲン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ルイセキ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ワ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>平面走査、BIT</t>
+    <rPh sb="0" eb="2">
+      <t>ヘイメン</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ソウサ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -583,11 +606,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C233B7-3D4E-4872-A3EB-9A4A81938CC3}">
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F130" sqref="F130"/>
+      <selection pane="bottomLeft" activeCell="F132" sqref="F132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2480,6 +2503,46 @@
       </c>
       <c r="F129" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A130">
+        <v>105</v>
+      </c>
+      <c r="B130" t="s">
+        <v>19</v>
+      </c>
+      <c r="C130" t="s">
+        <v>8</v>
+      </c>
+      <c r="D130" t="b">
+        <v>1</v>
+      </c>
+      <c r="E130" s="2">
+        <v>43713</v>
+      </c>
+      <c r="F130" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A131">
+        <v>105</v>
+      </c>
+      <c r="B131" t="s">
+        <v>19</v>
+      </c>
+      <c r="C131" t="s">
+        <v>8</v>
+      </c>
+      <c r="D131" t="b">
+        <v>1</v>
+      </c>
+      <c r="E131" s="2">
+        <v>43714</v>
+      </c>
+      <c r="F131" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
doing ABC044 (C, D not yet)
</commit_message>
<xml_diff>
--- a/AtCoder_record.xlsx
+++ b/AtCoder_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\codes\AtCoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399384F5-E6C4-45F3-A299-72D95208DD8A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FF469C-5319-4390-AAF5-DA601166B3E0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7170" yWindow="4455" windowWidth="12255" windowHeight="11940" xr2:uid="{9B9A1409-A6B9-4D33-8F83-A064BA4B158C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="52">
   <si>
     <t>contest</t>
     <phoneticPr fontId="1"/>
@@ -216,13 +216,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>バグが取れない</t>
-    <rPh sb="3" eb="4">
-      <t>ト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>メモ化</t>
     <rPh sb="2" eb="3">
       <t>カ</t>
@@ -377,38 +370,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>コスト正の最大化問題はコスト負の最小化問題</t>
-    <rPh sb="3" eb="4">
-      <t>セイ</t>
-    </rPh>
-    <rPh sb="5" eb="8">
-      <t>サイダイカ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>モンダイ</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>フ</t>
-    </rPh>
-    <rPh sb="16" eb="19">
-      <t>サイショウカ</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>モンダイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>最小木</t>
-    <rPh sb="0" eb="2">
-      <t>サイショウ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>キ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>使わない場合のdp更新し忘れ</t>
     <rPh sb="0" eb="1">
       <t>ツカ</t>
@@ -459,6 +420,51 @@
   </si>
   <si>
     <t>DAG</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>むずーーい</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bellman-ford</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>コスト正の最大化問題はコスト負の最小化問題　bellman-fordの負経路検出はどれでも検出したらtrueを返してしまう</t>
+    <rPh sb="3" eb="4">
+      <t>セイ</t>
+    </rPh>
+    <rPh sb="5" eb="8">
+      <t>サイダイカ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>モンダイ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>フ</t>
+    </rPh>
+    <rPh sb="16" eb="19">
+      <t>サイショウカ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>モンダイ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>フ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>ケイロ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ケンシュツ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ケンシュツ</t>
+    </rPh>
+    <rPh sb="55" eb="56">
+      <t>カエ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -826,11 +832,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C233B7-3D4E-4872-A3EB-9A4A81938CC3}">
-  <dimension ref="A1:G141"/>
+  <dimension ref="A1:G142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E141" sqref="E141"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -850,7 +856,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
         <v>6</v>
@@ -1324,7 +1330,7 @@
         <v>43710</v>
       </c>
       <c r="F31" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.4">
@@ -1677,15 +1683,12 @@
         <v>10</v>
       </c>
       <c r="C53" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="E53" s="1">
-        <v>43716</v>
+        <v>43730</v>
       </c>
       <c r="F53" t="s">
-        <v>28</v>
-      </c>
-      <c r="G53" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1790,16 +1793,16 @@
         <v>10</v>
       </c>
       <c r="C60" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="D60" t="b">
         <v>1</v>
       </c>
       <c r="E60" s="1">
-        <v>43717</v>
+        <v>43729</v>
       </c>
       <c r="G60" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.4">
@@ -1844,7 +1847,7 @@
         <v>43718</v>
       </c>
       <c r="F63" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.4">
@@ -1934,10 +1937,10 @@
         <v>43718</v>
       </c>
       <c r="F69" t="s">
+        <v>29</v>
+      </c>
+      <c r="G69" t="s">
         <v>30</v>
-      </c>
-      <c r="G69" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.4">
@@ -1948,7 +1951,7 @@
         <v>10</v>
       </c>
       <c r="C70" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D70" t="b">
         <v>1</v>
@@ -1957,7 +1960,7 @@
         <v>43718</v>
       </c>
       <c r="G70" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.4">
@@ -2033,10 +2036,10 @@
         <v>43719</v>
       </c>
       <c r="F75" t="s">
+        <v>33</v>
+      </c>
+      <c r="G75" t="s">
         <v>34</v>
-      </c>
-      <c r="G75" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.4">
@@ -2095,7 +2098,7 @@
         <v>43719</v>
       </c>
       <c r="F79" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.4">
@@ -2275,7 +2278,7 @@
         <v>43720</v>
       </c>
       <c r="F91" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.4">
@@ -2418,7 +2421,7 @@
         <v>43725</v>
       </c>
       <c r="F101" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.4">
@@ -2435,7 +2438,7 @@
         <v>43725</v>
       </c>
       <c r="F102" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.4">
@@ -2545,7 +2548,7 @@
         <v>43726</v>
       </c>
       <c r="F109" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.4">
@@ -2621,10 +2624,10 @@
         <v>43726</v>
       </c>
       <c r="F114" t="s">
+        <v>41</v>
+      </c>
+      <c r="G114" t="s">
         <v>42</v>
-      </c>
-      <c r="G114" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.4">
@@ -2649,19 +2652,19 @@
         <v>10</v>
       </c>
       <c r="C116" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="D116" t="b">
         <v>1</v>
       </c>
       <c r="E116" s="1">
-        <v>43726</v>
+        <v>43730</v>
       </c>
       <c r="F116" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G116" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.4">
@@ -2692,7 +2695,7 @@
         <v>43727</v>
       </c>
       <c r="F118" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.4">
@@ -2740,7 +2743,7 @@
         <v>8</v>
       </c>
       <c r="G121" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.4">
@@ -2785,7 +2788,7 @@
         <v>43728</v>
       </c>
       <c r="G124" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.4">
@@ -2889,7 +2892,7 @@
         <v>43728</v>
       </c>
       <c r="F131" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.4">
@@ -2954,7 +2957,7 @@
         <v>43728</v>
       </c>
       <c r="F135" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.4">
@@ -2971,7 +2974,7 @@
         <v>43728</v>
       </c>
       <c r="F136" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.4">
@@ -3042,6 +3045,26 @@
       </c>
       <c r="E141" s="1">
         <v>43729</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A142">
+        <v>86</v>
+      </c>
+      <c r="B142" t="s">
+        <v>10</v>
+      </c>
+      <c r="C142" t="s">
+        <v>5</v>
+      </c>
+      <c r="D142" t="b">
+        <v>1</v>
+      </c>
+      <c r="E142" s="1">
+        <v>43729</v>
+      </c>
+      <c r="F142" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -3073,12 +3096,12 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
doing recent contest A-Ds
</commit_message>
<xml_diff>
--- a/AtCoder_record.xlsx
+++ b/AtCoder_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\codes\AtCoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA32C34-9C5C-45A5-BE9D-C0218E2C5AA1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CC9B67-B494-42CB-A9FD-408A744AC028}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2595" yWindow="1905" windowWidth="12255" windowHeight="11940" activeTab="2" xr2:uid="{9B9A1409-A6B9-4D33-8F83-A064BA4B158C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="50">
   <si>
     <t>contest</t>
     <phoneticPr fontId="1"/>
@@ -429,6 +429,24 @@
     <rPh sb="2" eb="4">
       <t>フクゲン</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>二次元累積和</t>
+    <rPh sb="0" eb="6">
+      <t>ニジゲンルイセキワ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>貪欲</t>
+    <rPh sb="0" eb="2">
+      <t>ドンヨク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>O( N/1 + N/2 + ... + N/N ) = O( N logN )</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1797,11 +1815,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD4F28B-BDE7-4DDA-A1A4-081797C8432F}">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E82" sqref="E82"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2826,7 +2844,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>118</v>
       </c>
@@ -2841,6 +2859,90 @@
       </c>
       <c r="E81" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A82">
+        <v>75</v>
+      </c>
+      <c r="B82" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" s="1">
+        <v>43734</v>
+      </c>
+      <c r="E82" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A83">
+        <v>138</v>
+      </c>
+      <c r="B83" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" s="1">
+        <v>43734</v>
+      </c>
+      <c r="E83" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A84">
+        <v>137</v>
+      </c>
+      <c r="B84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="1">
+        <v>43734</v>
+      </c>
+      <c r="E84" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A85">
+        <v>136</v>
+      </c>
+      <c r="B85" t="s">
+        <v>5</v>
+      </c>
+      <c r="C85" s="1">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A86">
+        <v>135</v>
+      </c>
+      <c r="B86" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="1">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A87">
+        <v>134</v>
+      </c>
+      <c r="B87" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="1">
+        <v>43734</v>
+      </c>
+      <c r="D87" t="b">
+        <v>1</v>
+      </c>
+      <c r="E87" t="s">
+        <v>35</v>
+      </c>
+      <c r="F87" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
doing ABC140 (except E)
</commit_message>
<xml_diff>
--- a/AtCoder_record.xlsx
+++ b/AtCoder_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\codes\AtCoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CC9B67-B494-42CB-A9FD-408A744AC028}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A115FD79-D4E5-43E9-9490-AD1E6CA08D49}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="1905" windowWidth="12255" windowHeight="11940" activeTab="2" xr2:uid="{9B9A1409-A6B9-4D33-8F83-A064BA4B158C}"/>
+    <workbookView xWindow="10890" yWindow="5700" windowWidth="12255" windowHeight="11940" activeTab="3" xr2:uid="{9B9A1409-A6B9-4D33-8F83-A064BA4B158C}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ABC-C'!$A$1:$F$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ABC-D'!$A$1:$F$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ABC-D'!$A$1:$F$73</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ABC-E, F'!$A$1:$G$145</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="53">
   <si>
     <t>contest</t>
     <phoneticPr fontId="1"/>
@@ -447,6 +447,39 @@
   </si>
   <si>
     <t>O( N/1 + N/2 + ... + N/N ) = O( N logN )</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>event</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>尺取り法</t>
+    <rPh sb="0" eb="2">
+      <t>シャクト</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>multisetの構築は遅い。Vectorを構築してソートした方が速い</t>
+    <rPh sb="9" eb="11">
+      <t>コウチク</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>オソ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>コウチク</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>ハヤ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -504,7 +537,7 @@
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -522,6 +555,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -530,6 +570,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1797,10 +1844,10 @@
   </autoFilter>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"WA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"AC"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1815,11 +1862,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD4F28B-BDE7-4DDA-A1A4-081797C8432F}">
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F88" sqref="F88"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2397,32 +2444,35 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A47">
-        <v>75</v>
+        <v>141</v>
       </c>
       <c r="B47" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C47" s="1">
         <v>43725</v>
       </c>
-      <c r="D47" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A48">
-        <v>141</v>
+        <v>60</v>
       </c>
       <c r="B48" t="s">
         <v>5</v>
       </c>
       <c r="C48" s="1">
-        <v>43725</v>
+        <v>43726</v>
+      </c>
+      <c r="D48" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A49">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B49" t="s">
         <v>5</v>
@@ -2430,16 +2480,10 @@
       <c r="C49" s="1">
         <v>43726</v>
       </c>
-      <c r="D49" t="b">
-        <v>1</v>
-      </c>
-      <c r="F49" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A50">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B50" t="s">
         <v>5</v>
@@ -2447,10 +2491,13 @@
       <c r="C50" s="1">
         <v>43726</v>
       </c>
+      <c r="D50" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A51">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B51" t="s">
         <v>5</v>
@@ -2458,24 +2505,27 @@
       <c r="C51" s="1">
         <v>43726</v>
       </c>
-      <c r="D51" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A52">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B52" t="s">
         <v>5</v>
       </c>
       <c r="C52" s="1">
-        <v>43726</v>
+        <v>43727</v>
+      </c>
+      <c r="D52" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A53">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B53" t="s">
         <v>5</v>
@@ -2483,16 +2533,10 @@
       <c r="C53" s="1">
         <v>43727</v>
       </c>
-      <c r="D53" t="b">
-        <v>1</v>
-      </c>
-      <c r="F53" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A54">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B54" t="s">
         <v>5</v>
@@ -2503,7 +2547,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A55">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B55" t="s">
         <v>5</v>
@@ -2514,18 +2558,18 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A56">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B56" t="s">
         <v>5</v>
       </c>
       <c r="C56" s="1">
-        <v>43727</v>
+        <v>43728</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A57">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B57" t="s">
         <v>5</v>
@@ -2536,7 +2580,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A58">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B58" t="s">
         <v>5</v>
@@ -2544,10 +2588,13 @@
       <c r="C58" s="1">
         <v>43728</v>
       </c>
+      <c r="D58" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A59">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B59" t="s">
         <v>5</v>
@@ -2555,13 +2602,10 @@
       <c r="C59" s="1">
         <v>43728</v>
       </c>
-      <c r="D59" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A60">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B60" t="s">
         <v>5</v>
@@ -2572,7 +2616,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A61">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="B61" t="s">
         <v>5</v>
@@ -2580,10 +2624,13 @@
       <c r="C61" s="1">
         <v>43728</v>
       </c>
+      <c r="D61" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A62">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B62" t="s">
         <v>5</v>
@@ -2591,13 +2638,13 @@
       <c r="C62" s="1">
         <v>43728</v>
       </c>
-      <c r="D62" t="b">
-        <v>1</v>
+      <c r="F62" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A63">
-        <v>76</v>
+        <v>128</v>
       </c>
       <c r="B63" t="s">
         <v>5</v>
@@ -2605,24 +2652,21 @@
       <c r="C63" s="1">
         <v>43728</v>
       </c>
-      <c r="F63" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A64">
-        <v>128</v>
+        <v>45</v>
       </c>
       <c r="B64" t="s">
         <v>5</v>
       </c>
       <c r="C64" s="1">
-        <v>43728</v>
+        <v>43729</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A65">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B65" t="s">
         <v>5</v>
@@ -2633,7 +2677,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A66">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B66" t="s">
         <v>5</v>
@@ -2644,7 +2688,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A67">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="B67" t="s">
         <v>5</v>
@@ -2652,10 +2696,13 @@
       <c r="C67" s="1">
         <v>43729</v>
       </c>
+      <c r="D67" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A68">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B68" t="s">
         <v>5</v>
@@ -2666,27 +2713,30 @@
       <c r="D68" t="b">
         <v>1</v>
       </c>
+      <c r="F68" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A69">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="B69" t="s">
         <v>5</v>
       </c>
       <c r="C69" s="1">
-        <v>43729</v>
+        <v>43730</v>
       </c>
       <c r="D69" t="b">
         <v>1</v>
       </c>
       <c r="F69" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A70">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="B70" t="s">
         <v>5</v>
@@ -2694,27 +2744,24 @@
       <c r="C70" s="1">
         <v>43730</v>
       </c>
-      <c r="D70" t="b">
-        <v>1</v>
-      </c>
-      <c r="F70" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A71">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="B71" t="s">
         <v>5</v>
       </c>
       <c r="C71" s="1">
-        <v>43730</v>
+        <v>43731</v>
+      </c>
+      <c r="E71" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A72">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B72" t="s">
         <v>5</v>
@@ -2723,12 +2770,12 @@
         <v>43731</v>
       </c>
       <c r="E72" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A73">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="B73" t="s">
         <v>5</v>
@@ -2736,13 +2783,16 @@
       <c r="C73" s="1">
         <v>43731</v>
       </c>
+      <c r="D73" t="b">
+        <v>1</v>
+      </c>
       <c r="E73" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A74">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="B74" t="s">
         <v>5</v>
@@ -2750,27 +2800,27 @@
       <c r="C74" s="1">
         <v>43731</v>
       </c>
-      <c r="D74" t="b">
-        <v>1</v>
-      </c>
-      <c r="E74" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A75">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B75" t="s">
         <v>5</v>
       </c>
       <c r="C75" s="1">
-        <v>43731</v>
+        <v>43732</v>
+      </c>
+      <c r="D75" t="b">
+        <v>1</v>
+      </c>
+      <c r="E75" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A76">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B76" t="s">
         <v>5</v>
@@ -2778,30 +2828,27 @@
       <c r="C76" s="1">
         <v>43732</v>
       </c>
-      <c r="D76" t="b">
-        <v>1</v>
-      </c>
       <c r="E76" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A77">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B77" t="s">
         <v>5</v>
       </c>
       <c r="C77" s="1">
-        <v>43732</v>
+        <v>43733</v>
       </c>
       <c r="E77" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A78">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B78" t="s">
         <v>5</v>
@@ -2810,12 +2857,12 @@
         <v>43733</v>
       </c>
       <c r="E78" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A79">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B79" t="s">
         <v>5</v>
@@ -2823,30 +2870,33 @@
       <c r="C79" s="1">
         <v>43733</v>
       </c>
+      <c r="D79" t="b">
+        <v>1</v>
+      </c>
       <c r="E79" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A80">
-        <v>34</v>
+        <v>118</v>
       </c>
       <c r="B80" t="s">
         <v>5</v>
       </c>
       <c r="C80" s="1">
-        <v>43733</v>
+        <v>43734</v>
       </c>
       <c r="D80" t="b">
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A81">
-        <v>118</v>
+        <v>75</v>
       </c>
       <c r="B81" t="s">
         <v>5</v>
@@ -2854,16 +2904,13 @@
       <c r="C81" s="1">
         <v>43734</v>
       </c>
-      <c r="D81" t="b">
-        <v>1</v>
-      </c>
       <c r="E81" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A82">
-        <v>75</v>
+        <v>138</v>
       </c>
       <c r="B82" t="s">
         <v>5</v>
@@ -2872,12 +2919,12 @@
         <v>43734</v>
       </c>
       <c r="E82" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A83">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B83" t="s">
         <v>5</v>
@@ -2886,12 +2933,12 @@
         <v>43734</v>
       </c>
       <c r="E83" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A84">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B84" t="s">
         <v>5</v>
@@ -2899,13 +2946,10 @@
       <c r="C84" s="1">
         <v>43734</v>
       </c>
-      <c r="E84" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A85">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B85" t="s">
         <v>5</v>
@@ -2916,7 +2960,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A86">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B86" t="s">
         <v>5</v>
@@ -2924,44 +2968,110 @@
       <c r="C86" s="1">
         <v>43734</v>
       </c>
+      <c r="D86" t="b">
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
+        <v>35</v>
+      </c>
+      <c r="F86" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A87">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B87" t="s">
         <v>5</v>
       </c>
       <c r="C87" s="1">
-        <v>43734</v>
-      </c>
-      <c r="D87" t="b">
-        <v>1</v>
-      </c>
-      <c r="E87" t="s">
-        <v>35</v>
-      </c>
-      <c r="F87" t="s">
-        <v>49</v>
+        <v>43735</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A88">
+        <v>127</v>
+      </c>
+      <c r="B88" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="1">
+        <v>43735</v>
+      </c>
+      <c r="E88" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A89">
+        <v>44</v>
+      </c>
+      <c r="B89" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="1">
+        <v>43735</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A90">
+        <v>131</v>
+      </c>
+      <c r="B90" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="1">
+        <v>43735</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A91">
+        <v>132</v>
+      </c>
+      <c r="B91" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="1">
+        <v>43735</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A92">
+        <v>133</v>
+      </c>
+      <c r="B92" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="1">
+        <v>43735</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F74" xr:uid="{7ACCF93B-ECB5-4549-90E8-0D5590BFF3B1}">
-    <sortState ref="A2:F74">
-      <sortCondition ref="C1:C74"/>
+  <autoFilter ref="A1:F73" xr:uid="{7ACCF93B-ECB5-4549-90E8-0D5590BFF3B1}">
+    <sortState ref="A2:F73">
+      <sortCondition ref="C1:C73"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+  <conditionalFormatting sqref="B93:B1048576 B1:B90">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"WA"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"AC"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B91:B92">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"WA"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"AC"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B74" xr:uid="{4831945C-B34C-4191-9D68-06B7CAA2EBFD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B73" xr:uid="{4831945C-B34C-4191-9D68-06B7CAA2EBFD}">
       <formula1>"AC, WA, TLE, Not Answered"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2974,9 +3084,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C233B7-3D4E-4872-A3EB-9A4A81938CC3}">
   <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3077,10 +3187,44 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D6" s="1"/>
+      <c r="A6">
+        <v>127</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>43735</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D7" s="1"/>
+      <c r="A7">
+        <v>140</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>43735</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D8" s="1"/>
@@ -3512,7 +3656,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:D1048576" xr:uid="{73954FCB-6CAE-4348-A109-7122C619CB33}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{73954FCB-6CAE-4348-A109-7122C619CB33}">
       <formula1>"AC, WA, TLE, Not Answered"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
doing ABC138 (done: E; not yet : F)
</commit_message>
<xml_diff>
--- a/AtCoder_record.xlsx
+++ b/AtCoder_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\codes\AtCoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A115FD79-D4E5-43E9-9490-AD1E6CA08D49}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FE941F-560D-4D57-A94F-4A48E64A3223}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10890" yWindow="5700" windowWidth="12255" windowHeight="11940" activeTab="3" xr2:uid="{9B9A1409-A6B9-4D33-8F83-A064BA4B158C}"/>
+    <workbookView xWindow="10710" yWindow="7125" windowWidth="12255" windowHeight="11940" activeTab="3" xr2:uid="{9B9A1409-A6B9-4D33-8F83-A064BA4B158C}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="53">
   <si>
     <t>contest</t>
     <phoneticPr fontId="1"/>
@@ -3086,7 +3086,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3227,7 +3227,18 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D8" s="1"/>
+      <c r="A8">
+        <v>136</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>43736</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D9" s="1"/>

</xml_diff>

<commit_message>
done ABC134, 137 E (notF)
</commit_message>
<xml_diff>
--- a/AtCoder_record.xlsx
+++ b/AtCoder_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\codes\AtCoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FE941F-560D-4D57-A94F-4A48E64A3223}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4714FCC4-CDC1-4C2E-9E55-619EF1BB2F61}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10710" yWindow="7125" windowWidth="12255" windowHeight="11940" activeTab="3" xr2:uid="{9B9A1409-A6B9-4D33-8F83-A064BA4B158C}"/>
+    <workbookView xWindow="9120" yWindow="8115" windowWidth="12255" windowHeight="11940" activeTab="3" xr2:uid="{9B9A1409-A6B9-4D33-8F83-A064BA4B158C}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="55">
   <si>
     <t>contest</t>
     <phoneticPr fontId="1"/>
@@ -479,6 +479,20 @@
     </rPh>
     <rPh sb="33" eb="34">
       <t>ハヤ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Bellman-Ford</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ループ検出の亜種</t>
+    <rPh sb="3" eb="5">
+      <t>ケンシュツ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>アシュ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -3086,7 +3100,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3241,10 +3255,38 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D9" s="1"/>
+      <c r="A9">
+        <v>137</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1">
+        <v>43736</v>
+      </c>
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D10" s="1"/>
+      <c r="A10">
+        <v>134</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1">
+        <v>43736</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D11" s="1"/>

</xml_diff>

<commit_message>
participate ABC142 and complete after contest
</commit_message>
<xml_diff>
--- a/AtCoder_record.xlsx
+++ b/AtCoder_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\codes\AtCoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4714FCC4-CDC1-4C2E-9E55-619EF1BB2F61}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2684FA3-FBE6-4ABF-96CE-DC1CA8A73110}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9120" yWindow="8115" windowWidth="12255" windowHeight="11940" activeTab="3" xr2:uid="{9B9A1409-A6B9-4D33-8F83-A064BA4B158C}"/>
+    <workbookView xWindow="9120" yWindow="8115" windowWidth="12255" windowHeight="11940" xr2:uid="{9B9A1409-A6B9-4D33-8F83-A064BA4B158C}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ABC-C'!$A$1:$F$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ABC-D'!$A$1:$F$73</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ABC-E, F'!$A$1:$G$145</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ABC-E, F'!$A$1:$G$144</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="57">
   <si>
     <t>contest</t>
     <phoneticPr fontId="1"/>
@@ -145,10 +145,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>WA</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>尺取りは広義単調増加でやるべし、じゃないとO(n^2)になる</t>
     <rPh sb="0" eb="1">
       <t>シャク</t>
@@ -493,6 +489,27 @@
     </rPh>
     <rPh sb="6" eb="8">
       <t>アシュ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>偏角ソート</t>
+    <rPh sb="0" eb="2">
+      <t>ヘンカク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>atan2(y, x)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dfs 閉路検出</t>
+    <rPh sb="4" eb="6">
+      <t>ヘイロ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ケンシュツ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -920,15 +937,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{602BCC14-ABD2-46B0-A7E7-BF34DB839E1B}">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="A6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -953,22 +970,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" t="s">
-        <v>34</v>
-      </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
         <v>36</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -1548,7 +1565,7 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.4">
@@ -1777,7 +1794,7 @@
         <v>43731</v>
       </c>
       <c r="E71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.4">
@@ -1791,7 +1808,7 @@
         <v>43731</v>
       </c>
       <c r="E72" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.4">
@@ -1847,7 +1864,7 @@
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1879,7 +1896,7 @@
   <dimension ref="A1:F92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
@@ -1892,19 +1909,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" t="s">
-        <v>34</v>
-      </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -2132,7 +2149,7 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.4">
@@ -2182,7 +2199,7 @@
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.4">
@@ -2279,7 +2296,7 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.4">
@@ -2348,7 +2365,7 @@
         <v>43719</v>
       </c>
       <c r="F37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.4">
@@ -2481,7 +2498,7 @@
         <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.4">
@@ -2534,7 +2551,7 @@
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.4">
@@ -2653,7 +2670,7 @@
         <v>43728</v>
       </c>
       <c r="F62" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.4">
@@ -2728,7 +2745,7 @@
         <v>1</v>
       </c>
       <c r="F68" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.4">
@@ -2745,7 +2762,7 @@
         <v>1</v>
       </c>
       <c r="F69" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.4">
@@ -2770,7 +2787,7 @@
         <v>43731</v>
       </c>
       <c r="E71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.4">
@@ -2784,7 +2801,7 @@
         <v>43731</v>
       </c>
       <c r="E72" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.4">
@@ -2801,7 +2818,7 @@
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.4">
@@ -2829,7 +2846,7 @@
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.4">
@@ -2843,7 +2860,7 @@
         <v>43732</v>
       </c>
       <c r="E76" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.4">
@@ -2857,7 +2874,7 @@
         <v>43733</v>
       </c>
       <c r="E77" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.4">
@@ -2871,7 +2888,7 @@
         <v>43733</v>
       </c>
       <c r="E78" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.4">
@@ -2888,7 +2905,7 @@
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.4">
@@ -2905,7 +2922,7 @@
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.4">
@@ -2919,7 +2936,7 @@
         <v>43734</v>
       </c>
       <c r="E81" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.4">
@@ -2947,7 +2964,7 @@
         <v>43734</v>
       </c>
       <c r="E83" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.4">
@@ -2986,10 +3003,10 @@
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F86" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.4">
@@ -3014,7 +3031,7 @@
         <v>43735</v>
       </c>
       <c r="E88" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.4">
@@ -3096,11 +3113,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C233B7-3D4E-4872-A3EB-9A4A81938CC3}">
-  <dimension ref="A1:G145"/>
+  <dimension ref="A1:G144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3123,7 +3140,7 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -3134,21 +3151,27 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1">
-        <v>43716</v>
+        <v>43710</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -3159,16 +3182,13 @@
       <c r="D3" s="1">
         <v>43710</v>
       </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -3177,15 +3197,15 @@
         <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>43710</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
+        <v>43725</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
@@ -3194,18 +3214,18 @@
         <v>5</v>
       </c>
       <c r="D5" s="1">
-        <v>43725</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
+        <v>43735</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -3213,36 +3233,33 @@
       <c r="D6" s="1">
         <v>43735</v>
       </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="1">
-        <v>43735</v>
-      </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" t="s">
-        <v>52</v>
+        <v>43736</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
@@ -3253,10 +3270,16 @@
       <c r="D8" s="1">
         <v>43736</v>
       </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
@@ -3267,19 +3290,13 @@
       <c r="D9" s="1">
         <v>43736</v>
       </c>
-      <c r="F9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -3287,12 +3304,46 @@
       <c r="D10" s="1">
         <v>43736</v>
       </c>
+      <c r="F10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D11" s="1"/>
+      <c r="A11">
+        <v>142</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1">
+        <v>43736</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D12" s="1"/>
+      <c r="A12">
+        <v>142</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>43736</v>
+      </c>
+      <c r="F12" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D13" s="1"/>
@@ -3690,13 +3741,10 @@
     <row r="144" spans="4:4" x14ac:dyDescent="0.4">
       <c r="D144" s="1"/>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.4">
-      <c r="D145" s="1"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:G145" xr:uid="{B044DDE4-FD9B-4332-A4FA-1E362B47FB20}">
-    <sortState ref="A2:G145">
-      <sortCondition descending="1" ref="B1:B145"/>
+  <autoFilter ref="A1:G144" xr:uid="{B044DDE4-FD9B-4332-A4FA-1E362B47FB20}">
+    <sortState ref="A2:G144">
+      <sortCondition descending="1" ref="B1:B144"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
doing ABC138 (upto E OK, F not yet)
</commit_message>
<xml_diff>
--- a/AtCoder_record.xlsx
+++ b/AtCoder_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\codes\AtCoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC28E26C-CA30-4A60-9021-4D84C42CA7F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2663227B-DA85-45CA-B0F6-FA0DD1948CDA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9120" yWindow="8115" windowWidth="12255" windowHeight="11940" activeTab="3" xr2:uid="{9B9A1409-A6B9-4D33-8F83-A064BA4B158C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="60">
   <si>
     <t>contest</t>
     <phoneticPr fontId="1"/>
@@ -524,6 +524,22 @@
     </rPh>
     <rPh sb="5" eb="6">
       <t>ワ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>〇文字目が絡むときのインデックスの扱いがややこしい</t>
+    <rPh sb="1" eb="3">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>メ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>カラ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>アツカ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -3131,7 +3147,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3397,7 +3413,27 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D15" s="1"/>
+      <c r="A15">
+        <v>138</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
+        <v>43737</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D16" s="1"/>

</xml_diff>